<commit_message>
ajout des stats descriptives sur lignes et entetes
</commit_message>
<xml_diff>
--- a/temp.xlsx
+++ b/temp.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="43">
   <si>
     <t>Statistiques sur ARTICLES</t>
   </si>
@@ -74,12 +74,6 @@
     <t>PAYS</t>
   </si>
   <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>2</t>
-  </si>
-  <si>
     <t>DATEDEBUTADHESION</t>
   </si>
   <si>
@@ -96,6 +90,57 @@
   </si>
   <si>
     <t>Maximum</t>
+  </si>
+  <si>
+    <t>Statistiques sur SUBENTETE</t>
+  </si>
+  <si>
+    <t>X.ff..fe.IDTICKET</t>
+  </si>
+  <si>
+    <t>MAG_CODE</t>
+  </si>
+  <si>
+    <t>IDCLIENT</t>
+  </si>
+  <si>
+    <t>TIC_DATE</t>
+  </si>
+  <si>
+    <t>TIC_TOTALTTC</t>
+  </si>
+  <si>
+    <t>Effectif</t>
+  </si>
+  <si>
+    <t>Min1</t>
+  </si>
+  <si>
+    <t>Max1</t>
+  </si>
+  <si>
+    <t>Moyenne</t>
+  </si>
+  <si>
+    <t>Mediane</t>
+  </si>
+  <si>
+    <t>Ecart type</t>
+  </si>
+  <si>
+    <t>coefficient de variation</t>
+  </si>
+  <si>
+    <t>QUANTITE</t>
+  </si>
+  <si>
+    <t>MONTANTREMISE</t>
+  </si>
+  <si>
+    <t>TOTAL</t>
+  </si>
+  <si>
+    <t>MARGESORTIE</t>
   </si>
 </sst>
 </file>
@@ -103,7 +148,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="m/d/yyyy"/>
+    <numFmt numFmtId="165" formatCode="m/d/yyyy"/>
   </numFmts>
   <fonts count="6">
     <font>
@@ -178,16 +223,16 @@
       <alignment wrapText="true"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
 </styleSheet>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:H33"/>
+  <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -408,49 +453,49 @@
     <row r="30">
       <c r="A30"/>
       <c r="B30" t="s" s="11">
+        <v>20</v>
+      </c>
+      <c r="C30" t="s" s="11">
+        <v>21</v>
+      </c>
+      <c r="D30" t="s" s="11">
         <v>22</v>
       </c>
-      <c r="C30" t="s" s="11">
+      <c r="E30" t="s" s="11">
         <v>23</v>
-      </c>
-      <c r="D30" t="s" s="11">
-        <v>24</v>
-      </c>
-      <c r="E30" t="s" s="11">
-        <v>25</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s" s="8">
-        <v>26</v>
-      </c>
-      <c r="B31" t="n" s="15">
+        <v>24</v>
+      </c>
+      <c r="B31" t="n" s="13">
         <v>35813.0</v>
       </c>
-      <c r="C31" t="n" s="15">
+      <c r="C31" t="n" s="13">
         <v>39631.0</v>
       </c>
-      <c r="D31" t="n" s="15">
+      <c r="D31" t="n" s="13">
         <v>42400.0</v>
       </c>
-      <c r="E31" t="n" s="15">
+      <c r="E31" t="n" s="13">
         <v>-11364.0</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s" s="8">
-        <v>27</v>
-      </c>
-      <c r="B32" t="n" s="15">
+        <v>25</v>
+      </c>
+      <c r="B32" t="n" s="13">
         <v>43100.0</v>
       </c>
-      <c r="C32" t="n" s="15">
+      <c r="C32" t="n" s="13">
         <v>43107.0</v>
       </c>
-      <c r="D32" t="n" s="15">
+      <c r="D32" t="n" s="13">
         <v>71040.0</v>
       </c>
-      <c r="E32" t="n" s="15">
+      <c r="E32" t="n" s="13">
         <v>2218422.0</v>
       </c>
     </row>
@@ -458,17 +503,391 @@
       <c r="A33" t="s" s="8">
         <v>7</v>
       </c>
-      <c r="B33" t="n" s="15">
+      <c r="B33" t="n" s="13">
         <v>25569.0</v>
       </c>
-      <c r="C33" t="n" s="15">
+      <c r="C33" t="n" s="13">
         <v>25569.0</v>
       </c>
-      <c r="D33" t="n" s="15">
+      <c r="D33" t="n" s="13">
         <v>25569.0</v>
       </c>
-      <c r="E33" t="n" s="15">
+      <c r="E33" t="n" s="13">
         <v>25569.0</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="s" s="2">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="s" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42"/>
+      <c r="B42" t="s" s="11">
+        <v>27</v>
+      </c>
+      <c r="C42" t="s" s="11">
+        <v>28</v>
+      </c>
+      <c r="D42" t="s" s="11">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="s" s="8">
+        <v>6</v>
+      </c>
+      <c r="B43" t="n">
+        <v>67129.0</v>
+      </c>
+      <c r="C43" t="n">
+        <v>66.0</v>
+      </c>
+      <c r="D43" t="n">
+        <v>60108.0</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="s" s="8">
+        <v>7</v>
+      </c>
+      <c r="B44" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C44" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D44" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47"/>
+      <c r="B47" t="s" s="11">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="s" s="8">
+        <v>24</v>
+      </c>
+      <c r="B48" t="n" s="15">
+        <v>42371.0</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="s" s="8">
+        <v>25</v>
+      </c>
+      <c r="B49" t="n" s="15">
+        <v>43100.0</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="s" s="8">
+        <v>7</v>
+      </c>
+      <c r="B50" t="n" s="15">
+        <v>25569.0</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53"/>
+      <c r="B53" t="s" s="11">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="s" s="8">
+        <v>32</v>
+      </c>
+      <c r="B54" t="n">
+        <v>67129.0</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="s" s="8">
+        <v>24</v>
+      </c>
+      <c r="B55" t="n">
+        <v>-2636.38</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="s" s="8">
+        <v>33</v>
+      </c>
+      <c r="B56" t="n">
+        <v>-1907.9</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="s" s="8">
+        <v>25</v>
+      </c>
+      <c r="B57" t="n">
+        <v>3397.43</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="s" s="8">
+        <v>34</v>
+      </c>
+      <c r="B58" t="n">
+        <v>3364.32</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="s" s="8">
+        <v>35</v>
+      </c>
+      <c r="B59" t="n">
+        <v>58.5</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="s" s="8">
+        <v>36</v>
+      </c>
+      <c r="B60" t="n">
+        <v>37.7</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="s" s="8">
+        <v>37</v>
+      </c>
+      <c r="B61" t="n">
+        <v>88.2</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="s" s="8">
+        <v>38</v>
+      </c>
+      <c r="B62" t="n">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="s" s="8">
+        <v>7</v>
+      </c>
+      <c r="B63" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="s" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="s" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71"/>
+    </row>
+    <row r="72">
+      <c r="A72" t="s" s="8">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="s" s="8">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76"/>
+      <c r="B76" t="s" s="11">
+        <v>39</v>
+      </c>
+      <c r="C76" t="s" s="11">
+        <v>40</v>
+      </c>
+      <c r="D76" t="s" s="11">
+        <v>41</v>
+      </c>
+      <c r="E76" t="s" s="11">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="s" s="8">
+        <v>32</v>
+      </c>
+      <c r="B77" t="n">
+        <v>341322.0</v>
+      </c>
+      <c r="C77" t="n">
+        <v>341322.0</v>
+      </c>
+      <c r="D77" t="n">
+        <v>341322.0</v>
+      </c>
+      <c r="E77" t="n">
+        <v>341322.0</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="s" s="8">
+        <v>24</v>
+      </c>
+      <c r="B78" t="n">
+        <v>-40.0</v>
+      </c>
+      <c r="C78" t="n">
+        <v>-14.0</v>
+      </c>
+      <c r="D78" t="n">
+        <v>-1827.5</v>
+      </c>
+      <c r="E78" t="n">
+        <v>-1827.5</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="s" s="8">
+        <v>33</v>
+      </c>
+      <c r="B79" t="n">
+        <v>-20.0</v>
+      </c>
+      <c r="C79" t="n">
+        <v>-1.667</v>
+      </c>
+      <c r="D79" t="n">
+        <v>-1203.46</v>
+      </c>
+      <c r="E79" t="n">
+        <v>-720.99</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="s" s="8">
+        <v>25</v>
+      </c>
+      <c r="B80" t="n">
+        <v>188.0</v>
+      </c>
+      <c r="C80" t="n">
+        <v>1466.667</v>
+      </c>
+      <c r="D80" t="n">
+        <v>1979.25</v>
+      </c>
+      <c r="E80" t="n">
+        <v>958.33</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="s" s="8">
+        <v>34</v>
+      </c>
+      <c r="B81" t="n">
+        <v>170.0</v>
+      </c>
+      <c r="C81" t="n">
+        <v>707.242</v>
+      </c>
+      <c r="D81" t="n">
+        <v>1762.5</v>
+      </c>
+      <c r="E81" t="n">
+        <v>833.33</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="s" s="8">
+        <v>35</v>
+      </c>
+      <c r="B82" t="n">
+        <v>1.3</v>
+      </c>
+      <c r="C82" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="D82" t="n">
+        <v>10.0</v>
+      </c>
+      <c r="E82" t="n">
+        <v>4.2</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="s" s="8">
+        <v>36</v>
+      </c>
+      <c r="B83" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="C83" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D83" t="n">
+        <v>5.21</v>
+      </c>
+      <c r="E83" t="n">
+        <v>2.27</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="s" s="8">
+        <v>37</v>
+      </c>
+      <c r="B84" t="n">
+        <v>2.2</v>
+      </c>
+      <c r="C84" t="n">
+        <v>5.8</v>
+      </c>
+      <c r="D84" t="n">
+        <v>23.5</v>
+      </c>
+      <c r="E84" t="n">
+        <v>10.6</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="s" s="8">
+        <v>38</v>
+      </c>
+      <c r="B85" t="n">
+        <v>1.7</v>
+      </c>
+      <c r="C85" t="n">
+        <v>5.9</v>
+      </c>
+      <c r="D85" t="n">
+        <v>2.4</v>
+      </c>
+      <c r="E85" t="n">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="s" s="8">
+        <v>7</v>
+      </c>
+      <c r="B86" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C86" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D86" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="E86" t="n">
+        <v>0.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Correction stat de base
</commit_message>
<xml_diff>
--- a/temp.xlsx
+++ b/temp.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="46">
   <si>
     <t>Statistiques sur ARTICLES</t>
   </si>
@@ -129,6 +129,15 @@
   </si>
   <si>
     <t>coefficient de variation</t>
+  </si>
+  <si>
+    <t>Statistiques sur Sub Ligne</t>
+  </si>
+  <si>
+    <t>NUMLIGNETICKET</t>
+  </si>
+  <si>
+    <t>IDARTICLE</t>
   </si>
   <si>
     <t>QUANTITE</t>
@@ -684,7 +693,7 @@
     </row>
     <row r="66">
       <c r="A66" t="s" s="2">
-        <v>0</v>
+        <v>39</v>
       </c>
     </row>
     <row r="67">
@@ -694,30 +703,57 @@
     </row>
     <row r="71">
       <c r="A71"/>
+      <c r="B71" t="s" s="11">
+        <v>27</v>
+      </c>
+      <c r="C71" t="s" s="11">
+        <v>40</v>
+      </c>
+      <c r="D71" t="s" s="11">
+        <v>41</v>
+      </c>
     </row>
     <row r="72">
       <c r="A72" t="s" s="8">
         <v>6</v>
       </c>
+      <c r="B72" t="n">
+        <v>326361.0</v>
+      </c>
+      <c r="C72" t="n">
+        <v>92.0</v>
+      </c>
+      <c r="D72" t="n">
+        <v>49274.0</v>
+      </c>
     </row>
     <row r="73">
       <c r="A73" t="s" s="8">
         <v>7</v>
       </c>
+      <c r="B73" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C73" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="D73" t="n">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="76">
       <c r="A76"/>
       <c r="B76" t="s" s="11">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="C76" t="s" s="11">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="D76" t="s" s="11">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="E76" t="s" s="11">
-        <v>42</v>
+        <v>45</v>
       </c>
     </row>
     <row r="77">

</xml_diff>

<commit_message>
correction as factor false
</commit_message>
<xml_diff>
--- a/temp.xlsx
+++ b/temp.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="54">
   <si>
     <t>Statistiques sur ARTICLES</t>
   </si>
@@ -20,7 +20,7 @@
     <t>Tableau descriptif</t>
   </si>
   <si>
-    <t>X.U.FEFF.CODEARTICLE</t>
+    <t>ï..CODEARTICLE</t>
   </si>
   <si>
     <t>CODEUNIVERS</t>
@@ -41,7 +41,7 @@
     <t>Statistiques sur MAGASIN</t>
   </si>
   <si>
-    <t>X.U.FEFF.CODESOCIETE</t>
+    <t>ï..CODESOCIETE</t>
   </si>
   <si>
     <t>VILLE</t>
@@ -56,7 +56,7 @@
     <t>Statistiques sur CLIENTS</t>
   </si>
   <si>
-    <t>X.ff..fe.IDCLIENT</t>
+    <t>IDCLIENT</t>
   </si>
   <si>
     <t>CIVILITE</t>
@@ -92,19 +92,43 @@
     <t>Maximum</t>
   </si>
   <si>
+    <t>1/01/1997 0:00:00</t>
+  </si>
+  <si>
+    <t>9/12/2017 0:00:00</t>
+  </si>
+  <si>
+    <t>1/01/2018 0:00:00</t>
+  </si>
+  <si>
+    <t>1/01/2100 0:00:00</t>
+  </si>
+  <si>
+    <t>9/09/2018 0:00:00</t>
+  </si>
+  <si>
+    <t>1/01/1900 0:00:00</t>
+  </si>
+  <si>
+    <t>9/12/1998 0:00:00</t>
+  </si>
+  <si>
     <t>Statistiques sur SUBENTETE</t>
   </si>
   <si>
-    <t>X.ff..fe.IDTICKET</t>
+    <t>IDTICKET</t>
   </si>
   <si>
     <t>MAG_CODE</t>
   </si>
   <si>
-    <t>IDCLIENT</t>
-  </si>
-  <si>
     <t>TIC_DATE</t>
+  </si>
+  <si>
+    <t>2016-01-02 08:58:18</t>
+  </si>
+  <si>
+    <t>2017-12-31 18:03:26</t>
   </si>
   <si>
     <t>TIC_TOTALTTC</t>
@@ -156,9 +180,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="m/d/yyyy"/>
-  </numFmts>
+  <numFmts count="0"/>
   <fonts count="6">
     <font>
       <sz val="11.0"/>
@@ -216,7 +238,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="true"/>
@@ -231,10 +253,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true">
       <alignment wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
 </styleSheet>
 </file>
@@ -418,7 +436,7 @@
         <v>6</v>
       </c>
       <c r="B26" t="n">
-        <v>8464.0</v>
+        <v>845876.0</v>
       </c>
       <c r="C26" t="n">
         <v>6.0</v>
@@ -430,10 +448,10 @@
         <v>2.0</v>
       </c>
       <c r="F26" t="n">
-        <v>2700.0</v>
+        <v>16127.0</v>
       </c>
       <c r="G26" t="n">
-        <v>5.0</v>
+        <v>49.0</v>
       </c>
     </row>
     <row r="27">
@@ -453,10 +471,10 @@
         <v>0.0</v>
       </c>
       <c r="F27" t="n">
-        <v>0.0</v>
+        <v>3.2417281019913085</v>
       </c>
       <c r="G27" t="n">
-        <v>0.0</v>
+        <v>3.5466191262076237E-4</v>
       </c>
     </row>
     <row r="30">
@@ -478,56 +496,71 @@
       <c r="A31" t="s" s="8">
         <v>24</v>
       </c>
-      <c r="B31" t="n" s="13">
-        <v>35813.0</v>
-      </c>
-      <c r="C31" t="n" s="13">
-        <v>39631.0</v>
-      </c>
-      <c r="D31" t="n" s="13">
-        <v>42400.0</v>
-      </c>
-      <c r="E31" t="n" s="13">
-        <v>-11364.0</v>
+      <c r="B31" t="s">
+        <v>26</v>
+      </c>
+      <c r="C31" t="s">
+        <v>28</v>
+      </c>
+      <c r="D31" t="s">
+        <v>29</v>
+      </c>
+      <c r="E31" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s" s="8">
         <v>25</v>
       </c>
-      <c r="B32" t="n" s="13">
-        <v>43100.0</v>
-      </c>
-      <c r="C32" t="n" s="13">
-        <v>43107.0</v>
-      </c>
-      <c r="D32" t="n" s="13">
-        <v>71040.0</v>
-      </c>
-      <c r="E32" t="n" s="13">
-        <v>2218422.0</v>
+      <c r="B32" t="s">
+        <v>27</v>
+      </c>
+      <c r="C32" t="s">
+        <v>27</v>
+      </c>
+      <c r="D32" t="s">
+        <v>30</v>
+      </c>
+      <c r="E32" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="33">
-      <c r="A33" t="s" s="8">
+      <c r="A33"/>
+      <c r="B33" t="s" s="11">
+        <v>20</v>
+      </c>
+      <c r="C33" t="s" s="11">
+        <v>21</v>
+      </c>
+      <c r="D33" t="s" s="11">
+        <v>22</v>
+      </c>
+      <c r="E33" t="s" s="11">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="s" s="8">
         <v>7</v>
       </c>
-      <c r="B33" t="n" s="13">
-        <v>25569.0</v>
-      </c>
-      <c r="C33" t="n" s="13">
-        <v>25569.0</v>
-      </c>
-      <c r="D33" t="n" s="13">
-        <v>25569.0</v>
-      </c>
-      <c r="E33" t="n" s="13">
-        <v>25569.0</v>
+      <c r="B34" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C34" t="n">
+        <v>39.96566872685831</v>
+      </c>
+      <c r="D34" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="E34" t="n">
+        <v>39.955501752029846</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s" s="2">
-        <v>26</v>
+        <v>33</v>
       </c>
     </row>
     <row r="38">
@@ -538,13 +571,13 @@
     <row r="42">
       <c r="A42"/>
       <c r="B42" t="s" s="11">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="C42" t="s" s="11">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="D42" t="s" s="11">
-        <v>29</v>
+        <v>14</v>
       </c>
     </row>
     <row r="43">
@@ -552,13 +585,13 @@
         <v>6</v>
       </c>
       <c r="B43" t="n">
-        <v>67129.0</v>
+        <v>6714173.0</v>
       </c>
       <c r="C43" t="n">
         <v>66.0</v>
       </c>
       <c r="D43" t="n">
-        <v>60108.0</v>
+        <v>770163.0</v>
       </c>
     </row>
     <row r="44">
@@ -578,45 +611,51 @@
     <row r="47">
       <c r="A47"/>
       <c r="B47" t="s" s="11">
-        <v>30</v>
+        <v>36</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s" s="8">
         <v>24</v>
       </c>
-      <c r="B48" t="n" s="15">
-        <v>42371.0</v>
+      <c r="B48" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s" s="8">
         <v>25</v>
       </c>
-      <c r="B49" t="n" s="15">
-        <v>43100.0</v>
+      <c r="B49" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="50">
-      <c r="A50" t="s" s="8">
+      <c r="A50"/>
+      <c r="B50" t="s" s="11">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="s" s="8">
         <v>7</v>
       </c>
-      <c r="B50" t="n" s="15">
-        <v>25569.0</v>
+      <c r="B51" t="n">
+        <v>0.0</v>
       </c>
     </row>
     <row r="53">
       <c r="A53"/>
       <c r="B53" t="s" s="11">
-        <v>31</v>
+        <v>39</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="s" s="8">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="B54" t="n">
-        <v>67129.0</v>
+        <v>6714173.0</v>
       </c>
     </row>
     <row r="55">
@@ -624,15 +663,15 @@
         <v>24</v>
       </c>
       <c r="B55" t="n">
-        <v>-2636.38</v>
+        <v>-4404.0</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="s" s="8">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="B56" t="n">
-        <v>-1907.9</v>
+        <v>-3171.63</v>
       </c>
     </row>
     <row r="57">
@@ -640,44 +679,44 @@
         <v>25</v>
       </c>
       <c r="B57" t="n">
-        <v>3397.43</v>
+        <v>15355.25</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="s" s="8">
-        <v>34</v>
+        <v>42</v>
       </c>
       <c r="B58" t="n">
-        <v>3364.32</v>
+        <v>8516.32</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="s" s="8">
-        <v>35</v>
+        <v>43</v>
       </c>
       <c r="B59" t="n">
-        <v>58.5</v>
+        <v>58.2</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="s" s="8">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="B60" t="n">
-        <v>37.7</v>
+        <v>37.6</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="s" s="8">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="B61" t="n">
-        <v>88.2</v>
+        <v>86.7</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="s" s="8">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="B62" t="n">
         <v>1.5</v>
@@ -693,7 +732,7 @@
     </row>
     <row r="66">
       <c r="A66" t="s" s="2">
-        <v>39</v>
+        <v>47</v>
       </c>
     </row>
     <row r="67">
@@ -704,13 +743,13 @@
     <row r="71">
       <c r="A71"/>
       <c r="B71" t="s" s="11">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="C71" t="s" s="11">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="D71" t="s" s="11">
-        <v>41</v>
+        <v>49</v>
       </c>
     </row>
     <row r="72">
@@ -718,13 +757,13 @@
         <v>6</v>
       </c>
       <c r="B72" t="n">
-        <v>326361.0</v>
+        <v>6713822.0</v>
       </c>
       <c r="C72" t="n">
-        <v>92.0</v>
+        <v>152.0</v>
       </c>
       <c r="D72" t="n">
-        <v>49274.0</v>
+        <v>134828.0</v>
       </c>
     </row>
     <row r="73">
@@ -744,33 +783,33 @@
     <row r="76">
       <c r="A76"/>
       <c r="B76" t="s" s="11">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="C76" t="s" s="11">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="D76" t="s" s="11">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="E76" t="s" s="11">
-        <v>45</v>
+        <v>53</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="s" s="8">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="B77" t="n">
-        <v>341322.0</v>
+        <v>3.4105705E7</v>
       </c>
       <c r="C77" t="n">
-        <v>341322.0</v>
+        <v>3.4105705E7</v>
       </c>
       <c r="D77" t="n">
-        <v>341322.0</v>
+        <v>3.4105705E7</v>
       </c>
       <c r="E77" t="n">
-        <v>341322.0</v>
+        <v>3.4105705E7</v>
       </c>
     </row>
     <row r="78">
@@ -778,33 +817,33 @@
         <v>24</v>
       </c>
       <c r="B78" t="n">
-        <v>-40.0</v>
+        <v>-155.0</v>
       </c>
       <c r="C78" t="n">
-        <v>-14.0</v>
+        <v>-426.942</v>
       </c>
       <c r="D78" t="n">
-        <v>-1827.5</v>
+        <v>-15000.0</v>
       </c>
       <c r="E78" t="n">
-        <v>-1827.5</v>
+        <v>-15000.0</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="s" s="8">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="B79" t="n">
-        <v>-20.0</v>
+        <v>-148.0</v>
       </c>
       <c r="C79" t="n">
-        <v>-1.667</v>
+        <v>-133.0</v>
       </c>
       <c r="D79" t="n">
-        <v>-1203.46</v>
+        <v>-3333.33</v>
       </c>
       <c r="E79" t="n">
-        <v>-720.99</v>
+        <v>-3333.33</v>
       </c>
     </row>
     <row r="80">
@@ -812,38 +851,38 @@
         <v>25</v>
       </c>
       <c r="B80" t="n">
-        <v>188.0</v>
+        <v>999.0</v>
       </c>
       <c r="C80" t="n">
-        <v>1466.667</v>
+        <v>13166.667</v>
       </c>
       <c r="D80" t="n">
-        <v>1979.25</v>
+        <v>15000.0</v>
       </c>
       <c r="E80" t="n">
-        <v>958.33</v>
+        <v>15000.0</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="s" s="8">
-        <v>34</v>
+        <v>42</v>
       </c>
       <c r="B81" t="n">
-        <v>170.0</v>
+        <v>500.0</v>
       </c>
       <c r="C81" t="n">
-        <v>707.242</v>
+        <v>3268.909</v>
       </c>
       <c r="D81" t="n">
-        <v>1762.5</v>
+        <v>5000.0</v>
       </c>
       <c r="E81" t="n">
-        <v>833.33</v>
+        <v>5000.0</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="s" s="8">
-        <v>35</v>
+        <v>43</v>
       </c>
       <c r="B82" t="n">
         <v>1.3</v>
@@ -852,7 +891,7 @@
         <v>1.0</v>
       </c>
       <c r="D82" t="n">
-        <v>10.0</v>
+        <v>9.9</v>
       </c>
       <c r="E82" t="n">
         <v>4.2</v>
@@ -860,7 +899,7 @@
     </row>
     <row r="83">
       <c r="A83" t="s" s="8">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="B83" t="n">
         <v>1.0</v>
@@ -872,41 +911,41 @@
         <v>5.21</v>
       </c>
       <c r="E83" t="n">
-        <v>2.27</v>
+        <v>2.26</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="s" s="8">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="B84" t="n">
-        <v>2.2</v>
+        <v>2.3</v>
       </c>
       <c r="C84" t="n">
-        <v>5.8</v>
+        <v>6.1</v>
       </c>
       <c r="D84" t="n">
-        <v>23.5</v>
+        <v>24.3</v>
       </c>
       <c r="E84" t="n">
-        <v>10.6</v>
+        <v>11.7</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="s" s="8">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="B85" t="n">
         <v>1.7</v>
       </c>
       <c r="C85" t="n">
-        <v>5.9</v>
+        <v>6.1</v>
       </c>
       <c r="D85" t="n">
         <v>2.4</v>
       </c>
       <c r="E85" t="n">
-        <v>2.5</v>
+        <v>2.8</v>
       </c>
     </row>
     <row r="86">

</xml_diff>